<commit_message>
AutoMount script stuff added in
</commit_message>
<xml_diff>
--- a/IP Addresses.xlsx
+++ b/IP Addresses.xlsx
@@ -5,7 +5,7 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="H:\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="G:\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="885" uniqueCount="301">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="899" uniqueCount="306">
   <si>
     <t>IP Reference Sheet</t>
   </si>
@@ -922,6 +922,21 @@
   </si>
   <si>
     <t>orcinus2.ucsd.edu</t>
+  </si>
+  <si>
+    <t>Jenny Trickey</t>
+  </si>
+  <si>
+    <t>DataProcessing6</t>
+  </si>
+  <si>
+    <t>Remote Access</t>
+  </si>
+  <si>
+    <t>Ashlyn Giddings</t>
+  </si>
+  <si>
+    <t>Eadoh Reshef</t>
   </si>
 </sst>
 </file>
@@ -1809,13 +1824,13 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:Y1005"/>
+  <dimension ref="A1:Y1011"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <pane xSplit="2" ySplit="2" topLeftCell="C84" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="2" ySplit="2" topLeftCell="C3" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="C1" sqref="C1"/>
       <selection pane="bottomLeft" activeCell="A3" sqref="A3"/>
-      <selection pane="bottomRight" activeCell="B110" sqref="B110"/>
+      <selection pane="bottomRight" activeCell="C110" sqref="C110"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="17.28515625" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -5924,156 +5939,94 @@
     <row r="106" spans="1:18" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A106" s="96"/>
       <c r="B106" s="21" t="s">
-        <v>295</v>
+        <v>116</v>
       </c>
       <c r="C106" s="21" t="s">
-        <v>172</v>
-      </c>
-      <c r="D106" s="21" t="s">
-        <v>296</v>
-      </c>
-      <c r="E106" s="21" t="s">
-        <v>22</v>
-      </c>
-      <c r="F106" s="21" t="s">
-        <v>297</v>
-      </c>
-      <c r="G106" s="21">
-        <v>873</v>
-      </c>
-      <c r="H106" s="21">
-        <v>5000</v>
-      </c>
-      <c r="I106" s="57" t="s">
-        <v>22</v>
-      </c>
-      <c r="J106" s="57" t="s">
-        <v>23</v>
-      </c>
-      <c r="K106" s="21" t="s">
-        <v>22</v>
-      </c>
-      <c r="L106" s="21" t="s">
-        <v>22</v>
-      </c>
-      <c r="M106" s="21" t="s">
-        <v>58</v>
-      </c>
-      <c r="N106" s="21" t="s">
-        <v>22</v>
-      </c>
-      <c r="O106" s="21" t="s">
-        <v>58</v>
-      </c>
-      <c r="P106" s="31">
-        <v>5</v>
-      </c>
-      <c r="Q106" s="21" t="s">
-        <v>272</v>
-      </c>
+        <v>301</v>
+      </c>
+      <c r="D106" s="21"/>
+      <c r="E106" s="21"/>
+      <c r="F106" s="21"/>
+      <c r="G106" s="21"/>
+      <c r="H106" s="21"/>
+      <c r="I106" s="57"/>
+      <c r="J106" s="57"/>
+      <c r="K106" s="21"/>
+      <c r="L106" s="21"/>
+      <c r="M106" s="21"/>
+      <c r="N106" s="21"/>
+      <c r="O106" s="21"/>
+      <c r="P106" s="31"/>
+      <c r="Q106" s="21"/>
       <c r="R106" s="31"/>
     </row>
     <row r="107" spans="1:18" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A107" s="100"/>
+      <c r="A107" s="96"/>
       <c r="B107" s="21" t="s">
-        <v>298</v>
+        <v>302</v>
       </c>
       <c r="C107" s="21" t="s">
-        <v>172</v>
-      </c>
-      <c r="D107" s="21" t="s">
-        <v>299</v>
-      </c>
-      <c r="E107" s="21" t="s">
-        <v>21</v>
-      </c>
-      <c r="F107" s="21" t="s">
-        <v>300</v>
-      </c>
-      <c r="G107" s="21" t="s">
-        <v>192</v>
-      </c>
-      <c r="H107" s="21">
-        <v>5000</v>
-      </c>
-      <c r="I107" s="57" t="s">
-        <v>22</v>
-      </c>
-      <c r="J107" s="57" t="s">
-        <v>23</v>
-      </c>
-      <c r="K107" s="21" t="s">
-        <v>22</v>
-      </c>
-      <c r="L107" s="21" t="s">
-        <v>22</v>
-      </c>
-      <c r="M107" s="21" t="s">
-        <v>58</v>
-      </c>
-      <c r="N107" s="21" t="s">
-        <v>67</v>
-      </c>
-      <c r="O107" s="21" t="s">
-        <v>58</v>
-      </c>
-      <c r="P107" s="31">
-        <v>5</v>
-      </c>
-      <c r="Q107" s="21" t="s">
-        <v>192</v>
-      </c>
+        <v>303</v>
+      </c>
+      <c r="D107" s="21"/>
+      <c r="E107" s="21"/>
+      <c r="F107" s="21"/>
+      <c r="G107" s="21"/>
+      <c r="H107" s="21"/>
+      <c r="I107" s="57"/>
+      <c r="J107" s="57"/>
+      <c r="K107" s="21"/>
+      <c r="L107" s="21"/>
+      <c r="M107" s="21"/>
+      <c r="N107" s="21"/>
+      <c r="O107" s="21"/>
+      <c r="P107" s="31"/>
+      <c r="Q107" s="21"/>
       <c r="R107" s="31"/>
     </row>
-    <row r="108" spans="1:18" s="102" customFormat="1" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A108" s="99"/>
-      <c r="B108" s="99" t="s">
-        <v>173</v>
-      </c>
-      <c r="C108" s="99"/>
-      <c r="D108" s="99" t="s">
-        <v>174</v>
-      </c>
-      <c r="E108" s="99"/>
-      <c r="F108" s="99"/>
-      <c r="G108" s="99"/>
-      <c r="H108" s="99"/>
-      <c r="I108" s="101"/>
-      <c r="J108" s="101" t="s">
-        <v>175</v>
-      </c>
-      <c r="K108" s="99"/>
-      <c r="L108" s="99"/>
-      <c r="M108" s="99"/>
-      <c r="N108" s="99"/>
-      <c r="O108" s="99"/>
-      <c r="P108" s="98"/>
-      <c r="Q108" s="99"/>
-      <c r="R108" s="98"/>
+    <row r="108" spans="1:18" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A108" s="51">
+        <v>232</v>
+      </c>
+      <c r="B108" s="51"/>
+      <c r="C108" s="51"/>
+      <c r="D108" s="51" t="s">
+        <v>82</v>
+      </c>
+      <c r="E108" s="51"/>
+      <c r="F108" s="51" t="s">
+        <v>82</v>
+      </c>
+      <c r="G108" s="51"/>
+      <c r="H108" s="51"/>
+      <c r="I108" s="52"/>
+      <c r="J108" s="52" t="s">
+        <v>82</v>
+      </c>
+      <c r="K108" s="21"/>
+      <c r="L108" s="21"/>
+      <c r="M108" s="21"/>
+      <c r="N108" s="21"/>
+      <c r="O108" s="21"/>
+      <c r="P108" s="31"/>
+      <c r="Q108" s="21"/>
+      <c r="R108" s="31"/>
     </row>
     <row r="109" spans="1:18" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A109" s="51">
-        <v>425</v>
-      </c>
-      <c r="B109" s="51" t="s">
-        <v>202</v>
-      </c>
-      <c r="C109" s="51" t="s">
-        <v>203</v>
-      </c>
-      <c r="D109" s="51" t="s">
-        <v>288</v>
-      </c>
-      <c r="E109" s="51"/>
-      <c r="F109" s="51" t="s">
-        <v>289</v>
-      </c>
-      <c r="G109" s="51"/>
-      <c r="H109" s="51"/>
-      <c r="I109" s="52"/>
-      <c r="J109" s="52" t="s">
-        <v>82</v>
-      </c>
+      <c r="A109" s="96"/>
+      <c r="B109" s="21" t="s">
+        <v>77</v>
+      </c>
+      <c r="C109" s="21" t="s">
+        <v>304</v>
+      </c>
+      <c r="D109" s="21"/>
+      <c r="E109" s="21"/>
+      <c r="F109" s="21"/>
+      <c r="G109" s="21"/>
+      <c r="H109" s="21"/>
+      <c r="I109" s="57"/>
+      <c r="J109" s="57"/>
       <c r="K109" s="21"/>
       <c r="L109" s="21"/>
       <c r="M109" s="21"/>
@@ -6084,207 +6037,209 @@
       <c r="R109" s="31"/>
     </row>
     <row r="110" spans="1:18" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A110" s="85"/>
+      <c r="A110" s="96"/>
       <c r="B110" s="21" t="s">
-        <v>286</v>
+        <v>77</v>
       </c>
       <c r="C110" s="21" t="s">
-        <v>287</v>
-      </c>
-      <c r="D110" s="21" t="s">
-        <v>46</v>
-      </c>
-      <c r="E110" s="21" t="s">
-        <v>21</v>
-      </c>
+        <v>305</v>
+      </c>
+      <c r="D110" s="21"/>
+      <c r="E110" s="21"/>
       <c r="F110" s="21"/>
-      <c r="G110" s="21">
-        <v>873</v>
-      </c>
-      <c r="H110" s="21">
-        <v>3391</v>
-      </c>
-      <c r="I110" s="57" t="s">
-        <v>22</v>
-      </c>
-      <c r="J110" s="57" t="s">
-        <v>23</v>
-      </c>
-      <c r="K110" s="21" t="s">
-        <v>22</v>
-      </c>
-      <c r="L110" s="85" t="s">
-        <v>21</v>
-      </c>
-      <c r="M110" s="85" t="s">
-        <v>77</v>
-      </c>
-      <c r="N110" s="21" t="s">
-        <v>22</v>
-      </c>
-      <c r="O110" s="21" t="s">
-        <v>58</v>
-      </c>
-      <c r="P110" s="31" t="s">
-        <v>264</v>
-      </c>
-      <c r="Q110" s="21" t="s">
-        <v>22</v>
-      </c>
+      <c r="G110" s="21"/>
+      <c r="H110" s="21"/>
+      <c r="I110" s="57"/>
+      <c r="J110" s="57"/>
+      <c r="K110" s="21"/>
+      <c r="L110" s="21"/>
+      <c r="M110" s="21"/>
+      <c r="N110" s="21"/>
+      <c r="O110" s="21"/>
+      <c r="P110" s="31"/>
+      <c r="Q110" s="21"/>
       <c r="R110" s="31"/>
     </row>
     <row r="111" spans="1:18" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A111" s="96"/>
-      <c r="B111" s="21" t="s">
-        <v>290</v>
-      </c>
-      <c r="C111" s="21" t="s">
-        <v>291</v>
-      </c>
-      <c r="D111" s="21" t="s">
-        <v>275</v>
-      </c>
-      <c r="E111" s="21" t="s">
-        <v>21</v>
-      </c>
-      <c r="F111" s="21"/>
-      <c r="G111" s="21">
-        <v>5873</v>
-      </c>
-      <c r="H111" s="21">
-        <v>3390</v>
-      </c>
-      <c r="I111" s="57" t="s">
-        <v>22</v>
-      </c>
-      <c r="J111" s="57" t="s">
-        <v>23</v>
-      </c>
-      <c r="K111" s="96" t="s">
-        <v>292</v>
-      </c>
-      <c r="L111" s="21" t="s">
-        <v>22</v>
-      </c>
-      <c r="M111" s="21" t="s">
-        <v>58</v>
-      </c>
-      <c r="N111" s="96" t="s">
-        <v>21</v>
-      </c>
-      <c r="O111" s="21" t="s">
-        <v>149</v>
-      </c>
-      <c r="P111" s="31">
-        <v>6</v>
-      </c>
-      <c r="Q111" s="21" t="s">
-        <v>22</v>
-      </c>
+      <c r="A111" s="51">
+        <v>232</v>
+      </c>
+      <c r="B111" s="51"/>
+      <c r="C111" s="51"/>
+      <c r="D111" s="51" t="s">
+        <v>82</v>
+      </c>
+      <c r="E111" s="51"/>
+      <c r="F111" s="51" t="s">
+        <v>82</v>
+      </c>
+      <c r="G111" s="51"/>
+      <c r="H111" s="51"/>
+      <c r="I111" s="52"/>
+      <c r="J111" s="52" t="s">
+        <v>82</v>
+      </c>
+      <c r="K111" s="21"/>
+      <c r="L111" s="21"/>
+      <c r="M111" s="21"/>
+      <c r="N111" s="21"/>
+      <c r="O111" s="21"/>
+      <c r="P111" s="31"/>
+      <c r="Q111" s="21"/>
       <c r="R111" s="31"/>
     </row>
     <row r="112" spans="1:18" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A112" s="96"/>
       <c r="B112" s="21" t="s">
-        <v>293</v>
+        <v>295</v>
       </c>
       <c r="C112" s="21" t="s">
-        <v>294</v>
+        <v>172</v>
       </c>
       <c r="D112" s="21" t="s">
-        <v>151</v>
+        <v>296</v>
       </c>
       <c r="E112" s="21" t="s">
-        <v>77</v>
-      </c>
-      <c r="F112" s="21"/>
-      <c r="G112" s="21"/>
-      <c r="H112" s="21"/>
-      <c r="I112" s="57"/>
-      <c r="J112" s="57"/>
-      <c r="K112" s="21"/>
-      <c r="L112" s="21"/>
-      <c r="M112" s="21"/>
-      <c r="N112" s="21"/>
-      <c r="O112" s="21"/>
-      <c r="P112" s="31"/>
-      <c r="Q112" s="21"/>
+        <v>22</v>
+      </c>
+      <c r="F112" s="21" t="s">
+        <v>297</v>
+      </c>
+      <c r="G112" s="21">
+        <v>873</v>
+      </c>
+      <c r="H112" s="21">
+        <v>5000</v>
+      </c>
+      <c r="I112" s="57" t="s">
+        <v>22</v>
+      </c>
+      <c r="J112" s="57" t="s">
+        <v>23</v>
+      </c>
+      <c r="K112" s="21" t="s">
+        <v>22</v>
+      </c>
+      <c r="L112" s="21" t="s">
+        <v>22</v>
+      </c>
+      <c r="M112" s="21" t="s">
+        <v>58</v>
+      </c>
+      <c r="N112" s="21" t="s">
+        <v>22</v>
+      </c>
+      <c r="O112" s="21" t="s">
+        <v>58</v>
+      </c>
+      <c r="P112" s="31">
+        <v>5</v>
+      </c>
+      <c r="Q112" s="21" t="s">
+        <v>272</v>
+      </c>
       <c r="R112" s="31"/>
     </row>
     <row r="113" spans="1:18" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A113" s="51" t="s">
-        <v>176</v>
-      </c>
-      <c r="B113" s="51"/>
-      <c r="C113" s="51"/>
-      <c r="D113" s="51" t="s">
+      <c r="A113" s="100"/>
+      <c r="B113" s="21" t="s">
+        <v>298</v>
+      </c>
+      <c r="C113" s="21" t="s">
+        <v>172</v>
+      </c>
+      <c r="D113" s="21" t="s">
+        <v>299</v>
+      </c>
+      <c r="E113" s="21" t="s">
+        <v>21</v>
+      </c>
+      <c r="F113" s="21" t="s">
+        <v>300</v>
+      </c>
+      <c r="G113" s="21" t="s">
+        <v>192</v>
+      </c>
+      <c r="H113" s="21">
+        <v>5000</v>
+      </c>
+      <c r="I113" s="57" t="s">
+        <v>22</v>
+      </c>
+      <c r="J113" s="57" t="s">
+        <v>23</v>
+      </c>
+      <c r="K113" s="21" t="s">
+        <v>22</v>
+      </c>
+      <c r="L113" s="21" t="s">
+        <v>22</v>
+      </c>
+      <c r="M113" s="21" t="s">
+        <v>58</v>
+      </c>
+      <c r="N113" s="21" t="s">
+        <v>67</v>
+      </c>
+      <c r="O113" s="21" t="s">
+        <v>58</v>
+      </c>
+      <c r="P113" s="31">
+        <v>5</v>
+      </c>
+      <c r="Q113" s="21" t="s">
+        <v>192</v>
+      </c>
+      <c r="R113" s="31"/>
+    </row>
+    <row r="114" spans="1:18" s="102" customFormat="1" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A114" s="99"/>
+      <c r="B114" s="99" t="s">
+        <v>173</v>
+      </c>
+      <c r="C114" s="99"/>
+      <c r="D114" s="99" t="s">
+        <v>174</v>
+      </c>
+      <c r="E114" s="99"/>
+      <c r="F114" s="99"/>
+      <c r="G114" s="99"/>
+      <c r="H114" s="99"/>
+      <c r="I114" s="101"/>
+      <c r="J114" s="101" t="s">
+        <v>175</v>
+      </c>
+      <c r="K114" s="99"/>
+      <c r="L114" s="99"/>
+      <c r="M114" s="99"/>
+      <c r="N114" s="99"/>
+      <c r="O114" s="99"/>
+      <c r="P114" s="98"/>
+      <c r="Q114" s="99"/>
+      <c r="R114" s="98"/>
+    </row>
+    <row r="115" spans="1:18" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A115" s="51">
+        <v>425</v>
+      </c>
+      <c r="B115" s="51" t="s">
+        <v>202</v>
+      </c>
+      <c r="C115" s="51" t="s">
+        <v>203</v>
+      </c>
+      <c r="D115" s="51" t="s">
+        <v>288</v>
+      </c>
+      <c r="E115" s="51"/>
+      <c r="F115" s="51" t="s">
+        <v>289</v>
+      </c>
+      <c r="G115" s="51"/>
+      <c r="H115" s="51"/>
+      <c r="I115" s="52"/>
+      <c r="J115" s="52" t="s">
         <v>82</v>
-      </c>
-      <c r="E113" s="51"/>
-      <c r="F113" s="51" t="s">
-        <v>82</v>
-      </c>
-      <c r="G113" s="51"/>
-      <c r="H113" s="51"/>
-      <c r="I113" s="52"/>
-      <c r="J113" s="52" t="s">
-        <v>82</v>
-      </c>
-      <c r="K113" s="21"/>
-      <c r="L113" s="21"/>
-      <c r="M113" s="21"/>
-      <c r="N113" s="21"/>
-      <c r="O113" s="21"/>
-      <c r="P113" s="31"/>
-      <c r="Q113" s="21"/>
-      <c r="R113" s="31"/>
-    </row>
-    <row r="114" spans="1:18" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A114" s="21"/>
-      <c r="B114" s="21" t="s">
-        <v>177</v>
-      </c>
-      <c r="C114" s="21" t="s">
-        <v>35</v>
-      </c>
-      <c r="D114" s="21"/>
-      <c r="E114" s="21"/>
-      <c r="F114" s="21"/>
-      <c r="G114" s="21"/>
-      <c r="H114" s="21"/>
-      <c r="I114" s="57"/>
-      <c r="J114" s="57" t="s">
-        <v>51</v>
-      </c>
-      <c r="K114" s="21"/>
-      <c r="L114" s="21"/>
-      <c r="M114" s="21"/>
-      <c r="N114" s="21"/>
-      <c r="O114" s="21"/>
-      <c r="P114" s="31"/>
-      <c r="Q114" s="21"/>
-      <c r="R114" s="31"/>
-    </row>
-    <row r="115" spans="1:18" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A115" s="21"/>
-      <c r="B115" s="21" t="s">
-        <v>71</v>
-      </c>
-      <c r="C115" s="21" t="s">
-        <v>178</v>
-      </c>
-      <c r="D115" s="21" t="s">
-        <v>27</v>
-      </c>
-      <c r="E115" s="21"/>
-      <c r="F115" s="21"/>
-      <c r="G115" s="21">
-        <v>873</v>
-      </c>
-      <c r="H115" s="21"/>
-      <c r="I115" s="57"/>
-      <c r="J115" s="57" t="s">
-        <v>23</v>
       </c>
       <c r="K115" s="21"/>
       <c r="L115" s="21"/>
@@ -6296,63 +6251,119 @@
       <c r="R115" s="31"/>
     </row>
     <row r="116" spans="1:18" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A116" s="21" t="s">
-        <v>179</v>
-      </c>
-      <c r="B116" s="21"/>
-      <c r="C116" s="21"/>
+      <c r="A116" s="85"/>
+      <c r="B116" s="21" t="s">
+        <v>286</v>
+      </c>
+      <c r="C116" s="21" t="s">
+        <v>287</v>
+      </c>
       <c r="D116" s="21" t="s">
-        <v>180</v>
-      </c>
-      <c r="E116" s="21"/>
+        <v>46</v>
+      </c>
+      <c r="E116" s="21" t="s">
+        <v>21</v>
+      </c>
       <c r="F116" s="21"/>
-      <c r="G116" s="21" t="s">
-        <v>78</v>
-      </c>
-      <c r="H116" s="21"/>
-      <c r="I116" s="57"/>
-      <c r="J116" s="57"/>
-      <c r="K116" s="21"/>
-      <c r="L116" s="21"/>
-      <c r="M116" s="21"/>
-      <c r="N116" s="21"/>
-      <c r="O116" s="21"/>
-      <c r="P116" s="31"/>
-      <c r="Q116" s="21"/>
+      <c r="G116" s="21">
+        <v>873</v>
+      </c>
+      <c r="H116" s="21">
+        <v>3391</v>
+      </c>
+      <c r="I116" s="57" t="s">
+        <v>22</v>
+      </c>
+      <c r="J116" s="57" t="s">
+        <v>23</v>
+      </c>
+      <c r="K116" s="21" t="s">
+        <v>22</v>
+      </c>
+      <c r="L116" s="85" t="s">
+        <v>21</v>
+      </c>
+      <c r="M116" s="85" t="s">
+        <v>77</v>
+      </c>
+      <c r="N116" s="21" t="s">
+        <v>22</v>
+      </c>
+      <c r="O116" s="21" t="s">
+        <v>58</v>
+      </c>
+      <c r="P116" s="31" t="s">
+        <v>264</v>
+      </c>
+      <c r="Q116" s="21" t="s">
+        <v>22</v>
+      </c>
       <c r="R116" s="31"/>
     </row>
     <row r="117" spans="1:18" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A117" s="21">
-        <v>211</v>
-      </c>
+      <c r="A117" s="96"/>
       <c r="B117" s="21" t="s">
-        <v>166</v>
-      </c>
-      <c r="C117" s="21"/>
-      <c r="D117" s="21"/>
-      <c r="E117" s="21"/>
+        <v>290</v>
+      </c>
+      <c r="C117" s="21" t="s">
+        <v>291</v>
+      </c>
+      <c r="D117" s="21" t="s">
+        <v>275</v>
+      </c>
+      <c r="E117" s="21" t="s">
+        <v>21</v>
+      </c>
       <c r="F117" s="21"/>
-      <c r="G117" s="21"/>
-      <c r="H117" s="21"/>
-      <c r="I117" s="57"/>
-      <c r="J117" s="57"/>
-      <c r="K117" s="21"/>
-      <c r="L117" s="21"/>
-      <c r="M117" s="21"/>
-      <c r="N117" s="21"/>
-      <c r="O117" s="21"/>
-      <c r="P117" s="31"/>
-      <c r="Q117" s="21"/>
+      <c r="G117" s="21">
+        <v>5873</v>
+      </c>
+      <c r="H117" s="21">
+        <v>3390</v>
+      </c>
+      <c r="I117" s="57" t="s">
+        <v>22</v>
+      </c>
+      <c r="J117" s="57" t="s">
+        <v>23</v>
+      </c>
+      <c r="K117" s="96" t="s">
+        <v>292</v>
+      </c>
+      <c r="L117" s="21" t="s">
+        <v>22</v>
+      </c>
+      <c r="M117" s="21" t="s">
+        <v>58</v>
+      </c>
+      <c r="N117" s="96" t="s">
+        <v>21</v>
+      </c>
+      <c r="O117" s="21" t="s">
+        <v>149</v>
+      </c>
+      <c r="P117" s="31">
+        <v>6</v>
+      </c>
+      <c r="Q117" s="21" t="s">
+        <v>22</v>
+      </c>
       <c r="R117" s="31"/>
     </row>
     <row r="118" spans="1:18" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A118" s="21"/>
+      <c r="A118" s="96"/>
       <c r="B118" s="21" t="s">
-        <v>181</v>
-      </c>
-      <c r="C118" s="21"/>
-      <c r="D118" s="21"/>
-      <c r="E118" s="21"/>
+        <v>293</v>
+      </c>
+      <c r="C118" s="21" t="s">
+        <v>294</v>
+      </c>
+      <c r="D118" s="21" t="s">
+        <v>151</v>
+      </c>
+      <c r="E118" s="21" t="s">
+        <v>77</v>
+      </c>
       <c r="F118" s="21"/>
       <c r="G118" s="21"/>
       <c r="H118" s="21"/>
@@ -6368,20 +6379,24 @@
       <c r="R118" s="31"/>
     </row>
     <row r="119" spans="1:18" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A119" s="21">
-        <v>110</v>
-      </c>
-      <c r="B119" s="21" t="s">
-        <v>182</v>
-      </c>
-      <c r="C119" s="21"/>
-      <c r="D119" s="21"/>
-      <c r="E119" s="21"/>
-      <c r="F119" s="21"/>
-      <c r="G119" s="21"/>
-      <c r="H119" s="21"/>
-      <c r="I119" s="57"/>
-      <c r="J119" s="57"/>
+      <c r="A119" s="51" t="s">
+        <v>176</v>
+      </c>
+      <c r="B119" s="51"/>
+      <c r="C119" s="51"/>
+      <c r="D119" s="51" t="s">
+        <v>82</v>
+      </c>
+      <c r="E119" s="51"/>
+      <c r="F119" s="51" t="s">
+        <v>82</v>
+      </c>
+      <c r="G119" s="51"/>
+      <c r="H119" s="51"/>
+      <c r="I119" s="52"/>
+      <c r="J119" s="52" t="s">
+        <v>82</v>
+      </c>
       <c r="K119" s="21"/>
       <c r="L119" s="21"/>
       <c r="M119" s="21"/>
@@ -6394,16 +6409,20 @@
     <row r="120" spans="1:18" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A120" s="21"/>
       <c r="B120" s="21" t="s">
-        <v>183</v>
-      </c>
-      <c r="C120" s="21"/>
+        <v>177</v>
+      </c>
+      <c r="C120" s="21" t="s">
+        <v>35</v>
+      </c>
       <c r="D120" s="21"/>
       <c r="E120" s="21"/>
       <c r="F120" s="21"/>
       <c r="G120" s="21"/>
       <c r="H120" s="21"/>
       <c r="I120" s="57"/>
-      <c r="J120" s="57"/>
+      <c r="J120" s="57" t="s">
+        <v>51</v>
+      </c>
       <c r="K120" s="21"/>
       <c r="L120" s="21"/>
       <c r="M120" s="21"/>
@@ -6416,16 +6435,24 @@
     <row r="121" spans="1:18" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A121" s="21"/>
       <c r="B121" s="21" t="s">
-        <v>184</v>
-      </c>
-      <c r="C121" s="21"/>
-      <c r="D121" s="21"/>
+        <v>71</v>
+      </c>
+      <c r="C121" s="21" t="s">
+        <v>178</v>
+      </c>
+      <c r="D121" s="21" t="s">
+        <v>27</v>
+      </c>
       <c r="E121" s="21"/>
       <c r="F121" s="21"/>
-      <c r="G121" s="21"/>
+      <c r="G121" s="21">
+        <v>873</v>
+      </c>
       <c r="H121" s="21"/>
       <c r="I121" s="57"/>
-      <c r="J121" s="57"/>
+      <c r="J121" s="57" t="s">
+        <v>23</v>
+      </c>
       <c r="K121" s="21"/>
       <c r="L121" s="21"/>
       <c r="M121" s="21"/>
@@ -6436,17 +6463,19 @@
       <c r="R121" s="31"/>
     </row>
     <row r="122" spans="1:18" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A122" s="21">
-        <v>110</v>
-      </c>
-      <c r="B122" s="21" t="s">
-        <v>185</v>
-      </c>
+      <c r="A122" s="21" t="s">
+        <v>179</v>
+      </c>
+      <c r="B122" s="21"/>
       <c r="C122" s="21"/>
-      <c r="D122" s="21"/>
+      <c r="D122" s="21" t="s">
+        <v>180</v>
+      </c>
       <c r="E122" s="21"/>
       <c r="F122" s="21"/>
-      <c r="G122" s="21"/>
+      <c r="G122" s="21" t="s">
+        <v>78</v>
+      </c>
       <c r="H122" s="21"/>
       <c r="I122" s="57"/>
       <c r="J122" s="57"/>
@@ -6460,134 +6489,164 @@
       <c r="R122" s="31"/>
     </row>
     <row r="123" spans="1:18" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A123" s="6"/>
-      <c r="B123" s="5"/>
-      <c r="C123" s="5"/>
-      <c r="D123" s="3"/>
-      <c r="E123" s="3"/>
-      <c r="F123" s="6"/>
-      <c r="G123" s="3"/>
-      <c r="H123" s="3"/>
-      <c r="I123" s="7"/>
-      <c r="J123" s="8"/>
-      <c r="K123" s="3"/>
-      <c r="L123" s="3"/>
-      <c r="M123" s="3"/>
+      <c r="A123" s="21">
+        <v>211</v>
+      </c>
+      <c r="B123" s="21" t="s">
+        <v>166</v>
+      </c>
+      <c r="C123" s="21"/>
+      <c r="D123" s="21"/>
+      <c r="E123" s="21"/>
+      <c r="F123" s="21"/>
+      <c r="G123" s="21"/>
+      <c r="H123" s="21"/>
+      <c r="I123" s="57"/>
+      <c r="J123" s="57"/>
+      <c r="K123" s="21"/>
+      <c r="L123" s="21"/>
+      <c r="M123" s="21"/>
       <c r="N123" s="21"/>
       <c r="O123" s="21"/>
       <c r="P123" s="31"/>
-      <c r="Q123" s="3"/>
-      <c r="R123" s="4"/>
+      <c r="Q123" s="21"/>
+      <c r="R123" s="31"/>
     </row>
     <row r="124" spans="1:18" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A124" s="2"/>
-      <c r="B124" s="10"/>
-      <c r="C124" s="10"/>
-      <c r="D124" s="1"/>
-      <c r="E124" s="1"/>
-      <c r="F124" s="2"/>
-      <c r="G124" s="1"/>
-      <c r="H124" s="1"/>
-      <c r="I124" s="1"/>
-      <c r="J124" s="11"/>
-      <c r="K124" s="12"/>
-      <c r="L124" s="1"/>
-      <c r="M124" s="1"/>
-      <c r="N124" s="2"/>
-      <c r="O124" s="2"/>
-      <c r="Q124" s="1"/>
+      <c r="A124" s="21"/>
+      <c r="B124" s="21" t="s">
+        <v>181</v>
+      </c>
+      <c r="C124" s="21"/>
+      <c r="D124" s="21"/>
+      <c r="E124" s="21"/>
+      <c r="F124" s="21"/>
+      <c r="G124" s="21"/>
+      <c r="H124" s="21"/>
+      <c r="I124" s="57"/>
+      <c r="J124" s="57"/>
+      <c r="K124" s="21"/>
+      <c r="L124" s="21"/>
+      <c r="M124" s="21"/>
+      <c r="N124" s="21"/>
+      <c r="O124" s="21"/>
+      <c r="P124" s="31"/>
+      <c r="Q124" s="21"/>
+      <c r="R124" s="31"/>
     </row>
     <row r="125" spans="1:18" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A125" s="2"/>
-      <c r="B125" s="10"/>
-      <c r="C125" s="10"/>
-      <c r="D125" s="1"/>
-      <c r="E125" s="1"/>
-      <c r="F125" s="2"/>
-      <c r="G125" s="1"/>
-      <c r="H125" s="1"/>
-      <c r="I125" s="1"/>
-      <c r="J125" s="11"/>
-      <c r="K125" s="1"/>
-      <c r="L125" s="1"/>
-      <c r="M125" s="1"/>
-      <c r="N125" s="2"/>
-      <c r="O125" s="2"/>
-      <c r="Q125" s="1"/>
+      <c r="A125" s="21">
+        <v>110</v>
+      </c>
+      <c r="B125" s="21" t="s">
+        <v>182</v>
+      </c>
+      <c r="C125" s="21"/>
+      <c r="D125" s="21"/>
+      <c r="E125" s="21"/>
+      <c r="F125" s="21"/>
+      <c r="G125" s="21"/>
+      <c r="H125" s="21"/>
+      <c r="I125" s="57"/>
+      <c r="J125" s="57"/>
+      <c r="K125" s="21"/>
+      <c r="L125" s="21"/>
+      <c r="M125" s="21"/>
+      <c r="N125" s="21"/>
+      <c r="O125" s="21"/>
+      <c r="P125" s="31"/>
+      <c r="Q125" s="21"/>
+      <c r="R125" s="31"/>
     </row>
     <row r="126" spans="1:18" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A126" s="2"/>
-      <c r="B126" s="10"/>
-      <c r="C126" s="10"/>
-      <c r="D126" s="1"/>
-      <c r="E126" s="1"/>
-      <c r="F126" s="2"/>
-      <c r="G126" s="1"/>
-      <c r="H126" s="1"/>
-      <c r="I126" s="1"/>
-      <c r="J126" s="11"/>
-      <c r="K126" s="1"/>
-      <c r="L126" s="1"/>
-      <c r="M126" s="1"/>
-      <c r="N126" s="2"/>
-      <c r="O126" s="2"/>
-      <c r="Q126" s="1"/>
+      <c r="A126" s="21"/>
+      <c r="B126" s="21" t="s">
+        <v>183</v>
+      </c>
+      <c r="C126" s="21"/>
+      <c r="D126" s="21"/>
+      <c r="E126" s="21"/>
+      <c r="F126" s="21"/>
+      <c r="G126" s="21"/>
+      <c r="H126" s="21"/>
+      <c r="I126" s="57"/>
+      <c r="J126" s="57"/>
+      <c r="K126" s="21"/>
+      <c r="L126" s="21"/>
+      <c r="M126" s="21"/>
+      <c r="N126" s="21"/>
+      <c r="O126" s="21"/>
+      <c r="P126" s="31"/>
+      <c r="Q126" s="21"/>
+      <c r="R126" s="31"/>
     </row>
     <row r="127" spans="1:18" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A127" s="2"/>
-      <c r="B127" s="10"/>
-      <c r="C127" s="10"/>
-      <c r="D127" s="1"/>
-      <c r="E127" s="1"/>
-      <c r="F127" s="2"/>
-      <c r="G127" s="1"/>
-      <c r="H127" s="1"/>
-      <c r="I127" s="1"/>
-      <c r="J127" s="11"/>
-      <c r="K127" s="1"/>
-      <c r="L127" s="1"/>
-      <c r="M127" s="1"/>
-      <c r="N127" s="2"/>
-      <c r="O127" s="2"/>
-      <c r="Q127" s="1"/>
+      <c r="A127" s="21"/>
+      <c r="B127" s="21" t="s">
+        <v>184</v>
+      </c>
+      <c r="C127" s="21"/>
+      <c r="D127" s="21"/>
+      <c r="E127" s="21"/>
+      <c r="F127" s="21"/>
+      <c r="G127" s="21"/>
+      <c r="H127" s="21"/>
+      <c r="I127" s="57"/>
+      <c r="J127" s="57"/>
+      <c r="K127" s="21"/>
+      <c r="L127" s="21"/>
+      <c r="M127" s="21"/>
+      <c r="N127" s="21"/>
+      <c r="O127" s="21"/>
+      <c r="P127" s="31"/>
+      <c r="Q127" s="21"/>
+      <c r="R127" s="31"/>
     </row>
     <row r="128" spans="1:18" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A128" s="2"/>
-      <c r="B128" s="10"/>
-      <c r="C128" s="10"/>
-      <c r="D128" s="1"/>
-      <c r="E128" s="1"/>
-      <c r="F128" s="2"/>
-      <c r="G128" s="1"/>
-      <c r="H128" s="1"/>
-      <c r="I128" s="1"/>
-      <c r="J128" s="11"/>
-      <c r="K128" s="1"/>
-      <c r="L128" s="1"/>
-      <c r="M128" s="1"/>
-      <c r="N128" s="2"/>
-      <c r="O128" s="2"/>
-      <c r="Q128" s="1"/>
-    </row>
-    <row r="129" spans="1:17" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A129" s="2"/>
-      <c r="B129" s="10"/>
-      <c r="C129" s="10"/>
-      <c r="D129" s="1"/>
-      <c r="E129" s="1"/>
-      <c r="F129" s="2"/>
-      <c r="G129" s="1"/>
-      <c r="H129" s="1"/>
-      <c r="I129" s="1"/>
-      <c r="J129" s="11"/>
-      <c r="K129" s="1"/>
-      <c r="L129" s="1"/>
-      <c r="M129" s="1"/>
-      <c r="N129" s="2"/>
-      <c r="O129" s="2"/>
-      <c r="Q129" s="1"/>
-    </row>
-    <row r="130" spans="1:17" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A128" s="21">
+        <v>110</v>
+      </c>
+      <c r="B128" s="21" t="s">
+        <v>185</v>
+      </c>
+      <c r="C128" s="21"/>
+      <c r="D128" s="21"/>
+      <c r="E128" s="21"/>
+      <c r="F128" s="21"/>
+      <c r="G128" s="21"/>
+      <c r="H128" s="21"/>
+      <c r="I128" s="57"/>
+      <c r="J128" s="57"/>
+      <c r="K128" s="21"/>
+      <c r="L128" s="21"/>
+      <c r="M128" s="21"/>
+      <c r="N128" s="21"/>
+      <c r="O128" s="21"/>
+      <c r="P128" s="31"/>
+      <c r="Q128" s="21"/>
+      <c r="R128" s="31"/>
+    </row>
+    <row r="129" spans="1:18" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A129" s="6"/>
+      <c r="B129" s="5"/>
+      <c r="C129" s="5"/>
+      <c r="D129" s="3"/>
+      <c r="E129" s="3"/>
+      <c r="F129" s="6"/>
+      <c r="G129" s="3"/>
+      <c r="H129" s="3"/>
+      <c r="I129" s="7"/>
+      <c r="J129" s="8"/>
+      <c r="K129" s="3"/>
+      <c r="L129" s="3"/>
+      <c r="M129" s="3"/>
+      <c r="N129" s="21"/>
+      <c r="O129" s="21"/>
+      <c r="P129" s="31"/>
+      <c r="Q129" s="3"/>
+      <c r="R129" s="4"/>
+    </row>
+    <row r="130" spans="1:18" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A130" s="2"/>
       <c r="B130" s="10"/>
       <c r="C130" s="10"/>
@@ -6598,14 +6657,14 @@
       <c r="H130" s="1"/>
       <c r="I130" s="1"/>
       <c r="J130" s="11"/>
-      <c r="K130" s="1"/>
+      <c r="K130" s="12"/>
       <c r="L130" s="1"/>
       <c r="M130" s="1"/>
       <c r="N130" s="2"/>
       <c r="O130" s="2"/>
       <c r="Q130" s="1"/>
     </row>
-    <row r="131" spans="1:17" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="131" spans="1:18" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A131" s="2"/>
       <c r="B131" s="10"/>
       <c r="C131" s="10"/>
@@ -6623,7 +6682,7 @@
       <c r="O131" s="2"/>
       <c r="Q131" s="1"/>
     </row>
-    <row r="132" spans="1:17" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="132" spans="1:18" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A132" s="2"/>
       <c r="B132" s="10"/>
       <c r="C132" s="10"/>
@@ -6641,7 +6700,7 @@
       <c r="O132" s="2"/>
       <c r="Q132" s="1"/>
     </row>
-    <row r="133" spans="1:17" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="133" spans="1:18" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A133" s="2"/>
       <c r="B133" s="10"/>
       <c r="C133" s="10"/>
@@ -6659,7 +6718,7 @@
       <c r="O133" s="2"/>
       <c r="Q133" s="1"/>
     </row>
-    <row r="134" spans="1:17" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="134" spans="1:18" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A134" s="2"/>
       <c r="B134" s="10"/>
       <c r="C134" s="10"/>
@@ -6677,7 +6736,7 @@
       <c r="O134" s="2"/>
       <c r="Q134" s="1"/>
     </row>
-    <row r="135" spans="1:17" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="135" spans="1:18" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A135" s="2"/>
       <c r="B135" s="10"/>
       <c r="C135" s="10"/>
@@ -6695,7 +6754,7 @@
       <c r="O135" s="2"/>
       <c r="Q135" s="1"/>
     </row>
-    <row r="136" spans="1:17" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="136" spans="1:18" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A136" s="2"/>
       <c r="B136" s="10"/>
       <c r="C136" s="10"/>
@@ -6713,7 +6772,7 @@
       <c r="O136" s="2"/>
       <c r="Q136" s="1"/>
     </row>
-    <row r="137" spans="1:17" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="137" spans="1:18" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A137" s="2"/>
       <c r="B137" s="10"/>
       <c r="C137" s="10"/>
@@ -6731,7 +6790,7 @@
       <c r="O137" s="2"/>
       <c r="Q137" s="1"/>
     </row>
-    <row r="138" spans="1:17" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="138" spans="1:18" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A138" s="2"/>
       <c r="B138" s="10"/>
       <c r="C138" s="10"/>
@@ -6749,7 +6808,7 @@
       <c r="O138" s="2"/>
       <c r="Q138" s="1"/>
     </row>
-    <row r="139" spans="1:17" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="139" spans="1:18" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A139" s="2"/>
       <c r="B139" s="10"/>
       <c r="C139" s="10"/>
@@ -6767,7 +6826,7 @@
       <c r="O139" s="2"/>
       <c r="Q139" s="1"/>
     </row>
-    <row r="140" spans="1:17" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="140" spans="1:18" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A140" s="2"/>
       <c r="B140" s="10"/>
       <c r="C140" s="10"/>
@@ -6785,7 +6844,7 @@
       <c r="O140" s="2"/>
       <c r="Q140" s="1"/>
     </row>
-    <row r="141" spans="1:17" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="141" spans="1:18" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A141" s="2"/>
       <c r="B141" s="10"/>
       <c r="C141" s="10"/>
@@ -6803,7 +6862,7 @@
       <c r="O141" s="2"/>
       <c r="Q141" s="1"/>
     </row>
-    <row r="142" spans="1:17" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="142" spans="1:18" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A142" s="2"/>
       <c r="B142" s="10"/>
       <c r="C142" s="10"/>
@@ -6821,7 +6880,7 @@
       <c r="O142" s="2"/>
       <c r="Q142" s="1"/>
     </row>
-    <row r="143" spans="1:17" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="143" spans="1:18" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A143" s="2"/>
       <c r="B143" s="10"/>
       <c r="C143" s="10"/>
@@ -6839,7 +6898,7 @@
       <c r="O143" s="2"/>
       <c r="Q143" s="1"/>
     </row>
-    <row r="144" spans="1:17" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="144" spans="1:18" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A144" s="2"/>
       <c r="B144" s="10"/>
       <c r="C144" s="10"/>
@@ -22229,13 +22288,121 @@
       <c r="O998" s="2"/>
       <c r="Q998" s="1"/>
     </row>
-    <row r="999" spans="1:17" ht="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="1000" spans="1:17" ht="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="1001" spans="1:17" ht="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="1002" spans="1:17" ht="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="1003" spans="1:17" ht="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="1004" spans="1:17" ht="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="999" spans="1:17" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A999" s="2"/>
+      <c r="B999" s="10"/>
+      <c r="C999" s="10"/>
+      <c r="D999" s="1"/>
+      <c r="E999" s="1"/>
+      <c r="F999" s="2"/>
+      <c r="G999" s="1"/>
+      <c r="H999" s="1"/>
+      <c r="I999" s="1"/>
+      <c r="J999" s="11"/>
+      <c r="K999" s="1"/>
+      <c r="L999" s="1"/>
+      <c r="M999" s="1"/>
+      <c r="N999" s="2"/>
+      <c r="O999" s="2"/>
+      <c r="Q999" s="1"/>
+    </row>
+    <row r="1000" spans="1:17" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A1000" s="2"/>
+      <c r="B1000" s="10"/>
+      <c r="C1000" s="10"/>
+      <c r="D1000" s="1"/>
+      <c r="E1000" s="1"/>
+      <c r="F1000" s="2"/>
+      <c r="G1000" s="1"/>
+      <c r="H1000" s="1"/>
+      <c r="I1000" s="1"/>
+      <c r="J1000" s="11"/>
+      <c r="K1000" s="1"/>
+      <c r="L1000" s="1"/>
+      <c r="M1000" s="1"/>
+      <c r="N1000" s="2"/>
+      <c r="O1000" s="2"/>
+      <c r="Q1000" s="1"/>
+    </row>
+    <row r="1001" spans="1:17" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A1001" s="2"/>
+      <c r="B1001" s="10"/>
+      <c r="C1001" s="10"/>
+      <c r="D1001" s="1"/>
+      <c r="E1001" s="1"/>
+      <c r="F1001" s="2"/>
+      <c r="G1001" s="1"/>
+      <c r="H1001" s="1"/>
+      <c r="I1001" s="1"/>
+      <c r="J1001" s="11"/>
+      <c r="K1001" s="1"/>
+      <c r="L1001" s="1"/>
+      <c r="M1001" s="1"/>
+      <c r="N1001" s="2"/>
+      <c r="O1001" s="2"/>
+      <c r="Q1001" s="1"/>
+    </row>
+    <row r="1002" spans="1:17" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A1002" s="2"/>
+      <c r="B1002" s="10"/>
+      <c r="C1002" s="10"/>
+      <c r="D1002" s="1"/>
+      <c r="E1002" s="1"/>
+      <c r="F1002" s="2"/>
+      <c r="G1002" s="1"/>
+      <c r="H1002" s="1"/>
+      <c r="I1002" s="1"/>
+      <c r="J1002" s="11"/>
+      <c r="K1002" s="1"/>
+      <c r="L1002" s="1"/>
+      <c r="M1002" s="1"/>
+      <c r="N1002" s="2"/>
+      <c r="O1002" s="2"/>
+      <c r="Q1002" s="1"/>
+    </row>
+    <row r="1003" spans="1:17" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A1003" s="2"/>
+      <c r="B1003" s="10"/>
+      <c r="C1003" s="10"/>
+      <c r="D1003" s="1"/>
+      <c r="E1003" s="1"/>
+      <c r="F1003" s="2"/>
+      <c r="G1003" s="1"/>
+      <c r="H1003" s="1"/>
+      <c r="I1003" s="1"/>
+      <c r="J1003" s="11"/>
+      <c r="K1003" s="1"/>
+      <c r="L1003" s="1"/>
+      <c r="M1003" s="1"/>
+      <c r="N1003" s="2"/>
+      <c r="O1003" s="2"/>
+      <c r="Q1003" s="1"/>
+    </row>
+    <row r="1004" spans="1:17" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A1004" s="2"/>
+      <c r="B1004" s="10"/>
+      <c r="C1004" s="10"/>
+      <c r="D1004" s="1"/>
+      <c r="E1004" s="1"/>
+      <c r="F1004" s="2"/>
+      <c r="G1004" s="1"/>
+      <c r="H1004" s="1"/>
+      <c r="I1004" s="1"/>
+      <c r="J1004" s="11"/>
+      <c r="K1004" s="1"/>
+      <c r="L1004" s="1"/>
+      <c r="M1004" s="1"/>
+      <c r="N1004" s="2"/>
+      <c r="O1004" s="2"/>
+      <c r="Q1004" s="1"/>
+    </row>
     <row r="1005" spans="1:17" ht="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="1006" spans="1:17" ht="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="1007" spans="1:17" ht="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="1008" spans="1:17" ht="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="1009" ht="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="1010" ht="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="1011" ht="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
   </sheetData>
   <phoneticPr fontId="10" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>